<commit_message>
period band and phase status
</commit_message>
<xml_diff>
--- a/data/Marina_ciclo1.xlsx
+++ b/data/Marina_ciclo1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\merii\Desktop\onering\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F7128C-3F78-4BC0-BD77-A5AB10D5B7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDC3CB7-12ED-4D71-BB91-F76E6C69B4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{82AD3B1C-8EF9-48C3-ACFD-0DF909AD0632}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
   <si>
     <t>Fecha</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -403,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F05E82D-E3F5-416E-A588-5D51E69608FA}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A8" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -424,126 +427,108 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>45285</v>
-      </c>
-      <c r="B2">
-        <v>36</v>
+        <v>45279</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>45286</v>
-      </c>
-      <c r="B3">
-        <v>36</v>
+        <v>45280</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>45287</v>
-      </c>
-      <c r="B4">
-        <v>36</v>
+        <v>45281</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>45288</v>
-      </c>
-      <c r="B5">
-        <v>36.5</v>
+        <v>45282</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>45289</v>
-      </c>
-      <c r="B6">
-        <v>36.299999999999997</v>
+        <v>45283</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>45290</v>
-      </c>
-      <c r="B7">
-        <v>36.299999999999997</v>
+        <v>45284</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>45291</v>
+        <v>45285</v>
+      </c>
+      <c r="B8">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>45292</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
+        <v>45286</v>
+      </c>
+      <c r="B9">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>45293</v>
+        <v>45287</v>
       </c>
       <c r="B10">
         <v>36</v>
       </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>45294</v>
+        <v>45288</v>
       </c>
       <c r="B11">
-        <v>36.15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
+        <v>36.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>45295</v>
+        <v>45289</v>
       </c>
       <c r="B12">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
+        <v>36.299999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>45296</v>
+        <v>45290</v>
       </c>
       <c r="B13">
-        <v>36.15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
+        <v>36.299999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>45297</v>
-      </c>
-      <c r="B14">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>45298</v>
-      </c>
-      <c r="B15">
-        <v>36</v>
+        <v>45292</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -551,129 +536,195 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
+        <v>45293</v>
+      </c>
+      <c r="B16">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>45294</v>
+      </c>
+      <c r="B17">
+        <v>36.15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>45295</v>
+      </c>
+      <c r="B18">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>45296</v>
+      </c>
+      <c r="B19">
+        <v>36.15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>45297</v>
+      </c>
+      <c r="B20">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>45298</v>
+      </c>
+      <c r="B21">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
         <v>45299</v>
       </c>
-      <c r="B16">
+      <c r="B22">
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
         <v>45300</v>
       </c>
-      <c r="B17">
+      <c r="B23">
         <v>36.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
         <v>45301</v>
       </c>
-      <c r="B18">
+      <c r="B24">
         <v>36.450000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
         <v>45302</v>
       </c>
-      <c r="B19">
+      <c r="B25">
         <v>36.65</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
         <v>45303</v>
       </c>
-      <c r="B20">
+      <c r="B26">
         <v>36.65</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
         <v>45304</v>
-      </c>
-      <c r="B21">
-        <v>36.700000000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <v>45305</v>
-      </c>
-      <c r="B22">
-        <v>36.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <v>45306</v>
-      </c>
-      <c r="B23">
-        <v>36.700000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <v>45307</v>
-      </c>
-      <c r="B24">
-        <v>36.9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
-        <v>45308</v>
-      </c>
-      <c r="B25">
-        <v>36.6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
-        <v>45309</v>
-      </c>
-      <c r="B26">
-        <v>36.700000000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
-        <v>45310</v>
       </c>
       <c r="B27">
         <v>36.700000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>45311</v>
+        <v>45305</v>
       </c>
       <c r="B28">
         <v>36.6</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
+        <v>45306</v>
+      </c>
+      <c r="B29">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>45307</v>
+      </c>
+      <c r="B30">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>45308</v>
+      </c>
+      <c r="B31">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>45309</v>
+      </c>
+      <c r="B32">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>45310</v>
+      </c>
+      <c r="B33">
+        <v>36.700000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>45311</v>
+      </c>
+      <c r="B34">
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
         <v>45312</v>
       </c>
-      <c r="B29">
+      <c r="B35">
         <v>36.5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
         <v>45313</v>
       </c>
-      <c r="B30">
+      <c r="B36">
         <v>36.6</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
         <v>45314</v>
       </c>
-      <c r="B31">
+      <c r="B37">
         <v>36.200000000000003</v>
       </c>
     </row>

</xml_diff>